<commit_message>
add: congruent stimuli pairing
</commit_message>
<xml_diff>
--- a/GesturesIndividualStimuli.xlsx
+++ b/GesturesIndividualStimuli.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="gestures_all_files" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="gestures_combinations" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="112">
   <si>
     <t xml:space="preserve">GestureDescription</t>
   </si>
@@ -224,10 +225,140 @@
     <t xml:space="preserve">gg18</t>
   </si>
   <si>
+    <t xml:space="preserve">wave (both hands mixed)</t>
+  </si>
+  <si>
     <t xml:space="preserve">gg19</t>
   </si>
   <si>
     <t xml:space="preserve">gg20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Possible Combinations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg01-gg18; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg01-gg17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">negative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg01-gg09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg01-gg18; gg01-gg09; gg01-gg15;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg02-gg04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg02-gg19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg02-gg04; gg02-gg17; gg02-gg06; gg02-gg19;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg03-gg10;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg03-gg07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg03-gg07; gg03-gg09; gg03-gg10; gg03-gg15; gg03-gg19; gg03-gg20;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg04-gg11;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg04-gg15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg04-gg11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg04-gg06; gg04-gg09; gg04-gg15; gg04-gg18; gg04-gg19; gg04-gg20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg06-gg19;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">neutral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg06-gg13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg06-gg19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg06-gg08; gg06-gg10; gg06-gg13; gg06-gg17; gg06-gg20;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg07-gg10; gg07-gg19;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg08-gg20;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg08-gg19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg08-gg17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg08-gg17; gg08-gg19; gg08-gg20;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg09-gg15;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg09-gg10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg09-gg15; gg09-gg19; gg09-gg20;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg10-gg20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg10-gg17; gg10-gg18; gg10-gg19;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg11-gg18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg11-gg18; gg11-gg19; gg11-gg20;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg13-gg17;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg13-gg17; gg13-gg19; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg15-gg20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg15-gg19;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg17-gg19; gg17-gg20;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg18-gg20;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg19-gg20;</t>
   </si>
 </sst>
 </file>
@@ -237,7 +368,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -267,8 +398,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,13 +415,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBFBFBF"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA9D18E"/>
-        <bgColor rgb="FFBFBFBF"/>
+        <bgColor rgb="FFAFD095"/>
       </patternFill>
     </fill>
     <fill>
@@ -297,6 +434,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FFA9D18E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFBFBFBF"/>
       </patternFill>
     </fill>
   </fills>
@@ -338,7 +487,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -371,8 +520,28 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -410,7 +579,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -421,9 +590,9 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFA9D18E"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FFA9D18E"/>
+      <rgbColor rgb="FFAFD095"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
@@ -455,11 +624,11 @@
   </sheetPr>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -955,13 +1124,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1318,7 +1487,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
         <v>40</v>
       </c>
@@ -1336,69 +1505,89 @@
       </c>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="8" t="n">
+        <v>26</v>
+      </c>
+      <c r="D20" s="8" t="n">
+        <v>25</v>
+      </c>
+      <c r="E20" s="8" t="n">
+        <v>21</v>
+      </c>
+      <c r="F20" s="8" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="2" t="n">
-        <v>28</v>
-      </c>
-      <c r="D20" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="E20" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="F20" s="2" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C21" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="D21" s="2" t="n">
+      <c r="D22" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="E21" s="2" t="n">
+      <c r="E22" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="F21" s="2" t="n">
+      <c r="F22" s="2" t="n">
         <v>24</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-    </row>
-    <row r="24" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1409,4 +1598,558 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>